<commit_message>
Workbook series data source changed
</commit_message>
<xml_diff>
--- a/IWER/ER-Stat.xlsx
+++ b/IWER/ER-Stat.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>week</t>
   </si>
@@ -44,14 +44,17 @@
     <t>pneumonia + other age &lt; 1</t>
   </si>
   <si>
-    <t>pneumonia, total</t>
+    <t>https://www.health.gov.il/UnitsOffice/HD/PH/epidemiology/Pages/epidemiology_report.aspx</t>
+  </si>
+  <si>
+    <t>Grab reports here</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,6 +202,15 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
@@ -502,7 +514,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -545,11 +557,13 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -583,6 +597,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -848,10 +863,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'2020'!$B$2:$B$29</c:f>
+              <c:f>'2020'!$B$2:$B$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="52"/>
                 <c:pt idx="0">
                   <c:v>963</c:v>
                 </c:pt>
@@ -972,165 +987,165 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'2019'!$H$2:$H$53</c:f>
+              <c:f>'2019'!$F$2:$F$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>114</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>106</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>122</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>119</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>128</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>141</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>138</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>112</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>152</c:v>
+                  <c:v>132</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>109</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>144</c:v>
+                  <c:v>134</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>114</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>104</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>114</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="49">
                   <c:v>83</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>109</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>74</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>82</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>72</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="50">
                   <c:v>84</c:v>
                 </c:pt>
-                <c:pt idx="35">
-                  <c:v>74</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>91</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>82</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>115</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>106</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>111</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>94</c:v>
-                </c:pt>
                 <c:pt idx="51">
-                  <c:v>97</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1168,93 +1183,93 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'2020'!$H$2:$H$29</c:f>
+              <c:f>'2020'!$F$2:$F$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>99</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>151</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>130</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>134</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>125</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>136</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>103</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>51</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>51</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>51</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>77</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>136</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>100</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>133</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>113</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>89</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>92</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>95</c:v>
-                </c:pt>
                 <c:pt idx="25">
-                  <c:v>66</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>41</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>88</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2080,7 +2095,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="120" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2091,7 +2106,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9307286" cy="6086929"/>
+    <xdr:ext cx="9302750" cy="6080125"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -2377,10 +2392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2392,10 +2407,12 @@
     <col min="5" max="5" width="16.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" customWidth="1"/>
+    <col min="9" max="9" width="76.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2417,11 +2434,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2443,12 +2460,11 @@
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2">
-        <f>D2+E2+F2+G2</f>
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2470,12 +2486,8 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H53" si="0">D3+E3+F3+G3</f>
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2497,12 +2509,8 @@
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="H4">
-        <f t="shared" si="0"/>
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2524,12 +2532,8 @@
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5">
-        <f t="shared" si="0"/>
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2551,12 +2555,8 @@
       <c r="G6">
         <v>0</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2578,12 +2578,8 @@
       <c r="G7">
         <v>0</v>
       </c>
-      <c r="H7">
-        <f t="shared" si="0"/>
-        <v>141</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2605,12 +2601,8 @@
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2632,12 +2624,8 @@
       <c r="G9">
         <v>0</v>
       </c>
-      <c r="H9">
-        <f t="shared" si="0"/>
-        <v>112</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2659,12 +2647,8 @@
       <c r="G10">
         <v>0</v>
       </c>
-      <c r="H10">
-        <f t="shared" si="0"/>
-        <v>152</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2686,12 +2670,8 @@
       <c r="G11">
         <v>0</v>
       </c>
-      <c r="H11">
-        <f t="shared" si="0"/>
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2713,12 +2693,8 @@
       <c r="G12">
         <v>0</v>
       </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>144</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2740,12 +2716,8 @@
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="H13">
-        <f t="shared" si="0"/>
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2767,12 +2739,8 @@
       <c r="G14">
         <v>0</v>
       </c>
-      <c r="H14">
-        <f t="shared" si="0"/>
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2794,12 +2762,8 @@
       <c r="G15">
         <v>0</v>
       </c>
-      <c r="H15">
-        <f t="shared" si="0"/>
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2821,12 +2785,8 @@
       <c r="G16">
         <v>0</v>
       </c>
-      <c r="H16">
-        <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2848,12 +2808,8 @@
       <c r="G17">
         <v>0</v>
       </c>
-      <c r="H17">
-        <f t="shared" si="0"/>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2875,12 +2831,8 @@
       <c r="G18">
         <v>0</v>
       </c>
-      <c r="H18">
-        <f t="shared" si="0"/>
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2902,12 +2854,8 @@
       <c r="G19">
         <v>0</v>
       </c>
-      <c r="H19">
-        <f t="shared" si="0"/>
-        <v>109</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2929,12 +2877,8 @@
       <c r="G20">
         <v>0</v>
       </c>
-      <c r="H20">
-        <f t="shared" si="0"/>
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2956,12 +2900,8 @@
       <c r="G21">
         <v>0</v>
       </c>
-      <c r="H21">
-        <f t="shared" si="0"/>
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2983,12 +2923,8 @@
       <c r="G22">
         <v>0</v>
       </c>
-      <c r="H22">
-        <f t="shared" si="0"/>
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3010,12 +2946,8 @@
       <c r="G23">
         <v>0</v>
       </c>
-      <c r="H23">
-        <f t="shared" si="0"/>
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3037,12 +2969,8 @@
       <c r="G24">
         <v>0</v>
       </c>
-      <c r="H24">
-        <f t="shared" si="0"/>
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3064,12 +2992,8 @@
       <c r="G25">
         <v>0</v>
       </c>
-      <c r="H25">
-        <f t="shared" si="0"/>
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3091,12 +3015,8 @@
       <c r="G26">
         <v>0</v>
       </c>
-      <c r="H26">
-        <f t="shared" si="0"/>
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3118,12 +3038,8 @@
       <c r="G27">
         <v>0</v>
       </c>
-      <c r="H27">
-        <f t="shared" si="0"/>
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3145,12 +3061,8 @@
       <c r="G28">
         <v>0</v>
       </c>
-      <c r="H28">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3172,12 +3084,8 @@
       <c r="G29">
         <v>0</v>
       </c>
-      <c r="H29">
-        <f t="shared" si="0"/>
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3199,12 +3107,8 @@
       <c r="G30">
         <v>0</v>
       </c>
-      <c r="H30">
-        <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3226,12 +3130,8 @@
       <c r="G31">
         <v>0</v>
       </c>
-      <c r="H31">
-        <f t="shared" si="0"/>
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3253,12 +3153,8 @@
       <c r="G32">
         <v>0</v>
       </c>
-      <c r="H32">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3280,12 +3176,8 @@
       <c r="G33">
         <v>0</v>
       </c>
-      <c r="H33">
-        <f t="shared" si="0"/>
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3307,12 +3199,8 @@
       <c r="G34">
         <v>0</v>
       </c>
-      <c r="H34">
-        <f t="shared" si="0"/>
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3334,12 +3222,8 @@
       <c r="G35">
         <v>0</v>
       </c>
-      <c r="H35">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3361,12 +3245,8 @@
       <c r="G36">
         <v>0</v>
       </c>
-      <c r="H36">
-        <f t="shared" si="0"/>
-        <v>84</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3388,12 +3268,8 @@
       <c r="G37">
         <v>0</v>
       </c>
-      <c r="H37">
-        <f t="shared" si="0"/>
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3415,12 +3291,8 @@
       <c r="G38">
         <v>0</v>
       </c>
-      <c r="H38">
-        <f t="shared" si="0"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3442,12 +3314,8 @@
       <c r="G39">
         <v>0</v>
       </c>
-      <c r="H39">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3469,12 +3337,8 @@
       <c r="G40">
         <v>0</v>
       </c>
-      <c r="H40">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3496,12 +3360,8 @@
       <c r="G41">
         <v>0</v>
       </c>
-      <c r="H41">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3523,12 +3383,8 @@
       <c r="G42">
         <v>0</v>
       </c>
-      <c r="H42">
-        <f t="shared" si="0"/>
-        <v>79</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3550,12 +3406,8 @@
       <c r="G43">
         <v>0</v>
       </c>
-      <c r="H43">
-        <f t="shared" si="0"/>
-        <v>91</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3577,12 +3429,8 @@
       <c r="G44">
         <v>0</v>
       </c>
-      <c r="H44">
-        <f t="shared" si="0"/>
-        <v>73</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3604,12 +3452,8 @@
       <c r="G45">
         <v>0</v>
       </c>
-      <c r="H45">
-        <f t="shared" si="0"/>
-        <v>82</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3631,12 +3475,8 @@
       <c r="G46">
         <v>0</v>
       </c>
-      <c r="H46">
-        <f t="shared" si="0"/>
-        <v>115</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3658,12 +3498,8 @@
       <c r="G47">
         <v>0</v>
       </c>
-      <c r="H47">
-        <f t="shared" si="0"/>
-        <v>106</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3685,12 +3521,8 @@
       <c r="G48">
         <v>0</v>
       </c>
-      <c r="H48">
-        <f t="shared" si="0"/>
-        <v>79</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3712,12 +3544,8 @@
       <c r="G49">
         <v>0</v>
       </c>
-      <c r="H49">
-        <f t="shared" si="0"/>
-        <v>111</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3739,12 +3567,8 @@
       <c r="G50">
         <v>0</v>
       </c>
-      <c r="H50">
-        <f t="shared" si="0"/>
-        <v>92</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3766,12 +3590,8 @@
       <c r="G51">
         <v>0</v>
       </c>
-      <c r="H51">
-        <f t="shared" si="0"/>
-        <v>95</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3793,12 +3613,8 @@
       <c r="G52">
         <v>0</v>
       </c>
-      <c r="H52">
-        <f t="shared" si="0"/>
-        <v>94</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3819,26 +3635,25 @@
       </c>
       <c r="G53">
         <v>0</v>
-      </c>
-      <c r="H53">
-        <f t="shared" si="0"/>
-        <v>97</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:G53">
     <sortCondition ref="A2:A53"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="I1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3850,10 +3665,12 @@
     <col min="5" max="5" width="16.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.75" customWidth="1"/>
+    <col min="9" max="9" width="76.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3875,11 +3692,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3901,12 +3718,11 @@
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2">
-        <f>D2+E2+F2+G2</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3928,12 +3744,8 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H52" si="0">D3+E3+F3+G3</f>
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3955,12 +3767,8 @@
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="H4">
-        <f t="shared" si="0"/>
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3982,12 +3790,8 @@
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5">
-        <f t="shared" si="0"/>
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4009,12 +3813,8 @@
       <c r="G6">
         <v>0</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
-        <v>134</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4036,12 +3836,8 @@
       <c r="G7">
         <v>0</v>
       </c>
-      <c r="H7">
-        <f t="shared" si="0"/>
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4063,12 +3859,8 @@
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4090,12 +3882,8 @@
       <c r="G9">
         <v>0</v>
       </c>
-      <c r="H9">
-        <f t="shared" si="0"/>
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4117,12 +3905,8 @@
       <c r="G10">
         <v>0</v>
       </c>
-      <c r="H10">
-        <f t="shared" si="0"/>
-        <v>136</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4144,12 +3928,8 @@
       <c r="G11">
         <v>0</v>
       </c>
-      <c r="H11">
-        <f t="shared" si="0"/>
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4171,12 +3951,8 @@
       <c r="G12">
         <v>0</v>
       </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4198,12 +3974,8 @@
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="H13">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4225,12 +3997,8 @@
       <c r="G14">
         <v>0</v>
       </c>
-      <c r="H14">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4252,12 +4020,8 @@
       <c r="G15">
         <v>0</v>
       </c>
-      <c r="H15">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4279,12 +4043,8 @@
       <c r="G16">
         <v>0</v>
       </c>
-      <c r="H16">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4306,12 +4066,8 @@
       <c r="G17">
         <v>0</v>
       </c>
-      <c r="H17">
-        <f t="shared" si="0"/>
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4333,12 +4089,8 @@
       <c r="G18">
         <v>0</v>
       </c>
-      <c r="H18">
-        <f t="shared" si="0"/>
-        <v>136</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4360,12 +4112,8 @@
       <c r="G19">
         <v>0</v>
       </c>
-      <c r="H19">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4387,12 +4135,8 @@
       <c r="G20">
         <v>0</v>
       </c>
-      <c r="H20">
-        <f t="shared" si="0"/>
-        <v>133</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4414,12 +4158,8 @@
       <c r="G21">
         <v>0</v>
       </c>
-      <c r="H21">
-        <f t="shared" si="0"/>
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4441,12 +4181,8 @@
       <c r="G22">
         <v>0</v>
       </c>
-      <c r="H22">
-        <f t="shared" si="0"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4468,12 +4204,8 @@
       <c r="G23">
         <v>0</v>
       </c>
-      <c r="H23">
-        <f t="shared" si="0"/>
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4495,12 +4227,8 @@
       <c r="G24">
         <v>0</v>
       </c>
-      <c r="H24">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4522,12 +4250,8 @@
       <c r="G25">
         <v>0</v>
       </c>
-      <c r="H25">
-        <f t="shared" si="0"/>
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4549,12 +4273,8 @@
       <c r="G26">
         <v>0</v>
       </c>
-      <c r="H26">
-        <f t="shared" si="0"/>
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4576,12 +4296,8 @@
       <c r="G27">
         <v>0</v>
       </c>
-      <c r="H27">
-        <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4603,12 +4319,8 @@
       <c r="G28">
         <v>0</v>
       </c>
-      <c r="H28">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4628,148 +4340,6 @@
         <v>82</v>
       </c>
       <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="0"/>
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H33">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H34">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H40">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H41">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H42">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H43">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H44">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H45">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H46">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H48">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H50">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H51">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H52">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -4777,6 +4347,9 @@
   <sortState ref="A2:G29">
     <sortCondition ref="A2:A29"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="I1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>